<commit_message>
Added buildings & stuff
Title says all
</commit_message>
<xml_diff>
--- a/Documents/Design/Improvements_Buildings.xlsx
+++ b/Documents/Design/Improvements_Buildings.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Number of tiles</t>
   </si>
@@ -130,6 +130,18 @@
   </si>
   <si>
     <t>Siege workshop</t>
+  </si>
+  <si>
+    <t>Grocer</t>
+  </si>
+  <si>
+    <t>Apotecary</t>
+  </si>
+  <si>
+    <t>Mage guild</t>
+  </si>
+  <si>
+    <t>Mage tower</t>
   </si>
 </sst>
 </file>
@@ -475,11 +487,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
+      <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -616,59 +628,79 @@
         <v>26</v>
       </c>
     </row>
+    <row r="22" spans="2:2">
+      <c r="B22" t="s">
+        <v>38</v>
+      </c>
+    </row>
     <row r="23" spans="2:2">
       <c r="B23" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2">
-      <c r="B24" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="2:2">
       <c r="B25" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="2:2">
       <c r="B27" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2">
-      <c r="B28" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="2:2">
       <c r="B29" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2">
+      <c r="B30" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="2:2">
       <c r="B31" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2">
-      <c r="B32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="2:2">
       <c r="B33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="2:2">
       <c r="B34" t="s">
-        <v>37</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2">
+      <c r="B35" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="2:2">
       <c r="B36" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2">
+      <c r="B40" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2">
+      <c r="B41" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added priorities to buildings / improvements list
</commit_message>
<xml_diff>
--- a/Documents/Design/Improvements_Buildings.xlsx
+++ b/Documents/Design/Improvements_Buildings.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Improvements / Buildings</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>Elder council</t>
+  </si>
+  <si>
+    <t>Market</t>
   </si>
 </sst>
 </file>
@@ -211,11 +214,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -511,11 +514,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L46"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
+      <selection pane="bottomLeft" activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -542,7 +545,7 @@
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>42</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -571,6 +574,9 @@
       </c>
     </row>
     <row r="2" spans="1:12">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
@@ -601,7 +607,7 @@
       </c>
     </row>
     <row r="9" spans="1:12">
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C9" t="s">
@@ -609,25 +615,28 @@
       </c>
     </row>
     <row r="10" spans="1:12">
-      <c r="B10" s="2"/>
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" s="3"/>
       <c r="C10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:12">
-      <c r="B11" s="2"/>
+      <c r="B11" s="3"/>
       <c r="C11" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:12">
-      <c r="B12" s="2"/>
+      <c r="B12" s="3"/>
       <c r="C12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:12">
-      <c r="B13" s="2"/>
+      <c r="B13" s="3"/>
       <c r="C13" t="s">
         <v>17</v>
       </c>
@@ -702,59 +711,67 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="3:3">
+    <row r="33" spans="1:3">
       <c r="C33" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="3:3">
+    <row r="34" spans="1:3">
       <c r="C34" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="3:3">
+    <row r="35" spans="1:3">
       <c r="C35" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="3:3">
+    <row r="36" spans="1:3">
       <c r="C36" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="3:3">
+    <row r="38" spans="1:3">
       <c r="C38" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="3:3">
+    <row r="40" spans="1:3">
       <c r="C40" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="3:3">
+    <row r="41" spans="1:3">
       <c r="C41" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="3:3">
+    <row r="43" spans="1:3">
       <c r="C43" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="3:3">
+    <row r="44" spans="1:3">
       <c r="C44" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="3:3">
+    <row r="45" spans="1:3">
       <c r="C45" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="46" spans="3:3">
+    <row r="46" spans="1:3">
       <c r="C46" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tweaks excel de buildings
</commit_message>
<xml_diff>
--- a/Documents/Design/Improvements_Buildings.xlsx
+++ b/Documents/Design/Improvements_Buildings.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="55">
   <si>
     <t>Improvements / Buildings</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Habitation</t>
   </si>
   <si>
-    <t>Temple</t>
-  </si>
-  <si>
     <t>Monastery</t>
   </si>
   <si>
@@ -166,6 +163,24 @@
   </si>
   <si>
     <t>Market</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>in Engine</t>
+  </si>
+  <si>
+    <t>Chapel</t>
+  </si>
+  <si>
+    <t>Courthouse</t>
+  </si>
+  <si>
+    <t>Town Hall</t>
+  </si>
+  <si>
+    <t>Palace</t>
   </si>
 </sst>
 </file>
@@ -209,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -219,6 +234,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -514,270 +535,319 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L48"/>
+  <dimension ref="A1:M52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C49" sqref="C49"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.42578125" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="34.28515625" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" customWidth="1"/>
-    <col min="6" max="7" width="18.5703125" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" customWidth="1"/>
-    <col min="9" max="10" width="20.7109375" customWidth="1"/>
-    <col min="11" max="11" width="22.42578125" customWidth="1"/>
-    <col min="12" max="12" width="44.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" customWidth="1"/>
+    <col min="7" max="8" width="18.5703125" customWidth="1"/>
+    <col min="9" max="9" width="20.5703125" customWidth="1"/>
+    <col min="10" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="22.42578125" customWidth="1"/>
+    <col min="13" max="13" width="44.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="31.5" customHeight="1">
+    <row r="1" spans="1:13" ht="31.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:13">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
-      <c r="C3" t="s">
+    <row r="3" spans="1:13">
+      <c r="D3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
-      <c r="C4" t="s">
+    <row r="4" spans="1:13">
+      <c r="D4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
-      <c r="C5" t="s">
+    <row r="5" spans="1:13">
+      <c r="D5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
-      <c r="C6" t="s">
+    <row r="6" spans="1:13">
+      <c r="D6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
-      <c r="C7" t="s">
+    <row r="7" spans="1:13">
+      <c r="D7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:13">
       <c r="B9" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="5"/>
+      <c r="D9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:13">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" s="3"/>
-      <c r="C10" t="s">
+      <c r="C10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:13">
       <c r="B11" s="3"/>
-      <c r="C11" t="s">
+      <c r="C11" s="5"/>
+      <c r="D11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:13">
       <c r="B12" s="3"/>
-      <c r="C12" t="s">
+      <c r="C12" s="5"/>
+      <c r="D12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:13">
       <c r="B13" s="3"/>
-      <c r="C13" t="s">
+      <c r="C13" s="5"/>
+      <c r="D13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
-      <c r="C15" t="s">
+    <row r="15" spans="1:13">
+      <c r="D15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
-      <c r="C16" t="s">
+    <row r="16" spans="1:13">
+      <c r="C16" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4">
+      <c r="C17" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="3:3">
-      <c r="C17" t="s">
+    <row r="18" spans="3:4">
+      <c r="D18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="3:3">
-      <c r="C18" t="s">
+    <row r="20" spans="3:4">
+      <c r="D20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="3:3">
-      <c r="C20" t="s">
+    <row r="21" spans="3:4">
+      <c r="D21" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="3:3">
-      <c r="C21" t="s">
+    <row r="22" spans="3:4">
+      <c r="D22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="3:4">
+      <c r="D23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="3:4">
+      <c r="D25" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="3:3">
-      <c r="C22" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="3:3">
-      <c r="C23" t="s">
+    <row r="26" spans="3:4">
+      <c r="D26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="3:4">
+      <c r="D27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="3:4">
+      <c r="D29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="3:4">
+      <c r="D30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="3:4">
+      <c r="D31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="D33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="D34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="D35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="D36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="D38" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="D40" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="3:3">
-      <c r="C25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="3:3">
-      <c r="C26" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="3:3">
-      <c r="C27" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="3:3">
-      <c r="C29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="3:3">
-      <c r="C30" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="3:3">
-      <c r="C31" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="C33" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="C34" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="C35" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="C36" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="C38" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="C40" t="s">
+    <row r="41" spans="1:4">
+      <c r="D41" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
-      <c r="C41" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="C43" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="C44" t="s">
+    <row r="43" spans="1:4">
+      <c r="D43" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="C44" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D44" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="D45" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
-      <c r="C45" t="s">
+    <row r="46" spans="1:4">
+      <c r="C46" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D46" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
-      <c r="C46" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:4">
       <c r="A48">
         <v>1</v>
       </c>
-      <c r="C48" t="s">
-        <v>49</v>
+      <c r="D48" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4">
+      <c r="C50" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D50" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4">
+      <c r="D51" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4">
+      <c r="D52" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B9:B13"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C52">
+      <formula1>"Not started, In progress, 3D done, in Engine"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -787,9 +857,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+  </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>